<commit_message>
Added final price data for October 2022.
</commit_message>
<xml_diff>
--- a/price_data/data (103).xlsx
+++ b/price_data/data (103).xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
   <si>
     <t>Tidsperiod</t>
   </si>
@@ -306,6 +306,222 @@
   </si>
   <si>
     <t>2022-09-25 23:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 00:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 01:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 02:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 03:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 04:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 05:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 06:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 07:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 08:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 09:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 10:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 11:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 12:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 13:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 14:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 15:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 16:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 17:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 18:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 19:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 20:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 21:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 22:00</t>
+  </si>
+  <si>
+    <t>2022-09-26 23:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 00:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 01:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 02:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 03:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 04:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 05:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 06:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 07:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 08:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 09:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 10:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 11:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 12:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 13:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 14:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 15:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 16:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 17:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 18:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 19:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 20:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 21:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 22:00</t>
+  </si>
+  <si>
+    <t>2022-09-27 23:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 00:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 01:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 02:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 03:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 04:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 05:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 06:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 07:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 08:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 09:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 10:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 11:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 12:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 13:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 14:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 15:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 16:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 17:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 18:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 19:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 20:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 21:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 22:00</t>
+  </si>
+  <si>
+    <t>2022-09-28 23:00</t>
   </si>
 </sst>
 </file>
@@ -350,7 +566,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B98" headerRowCount="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:B170" headerRowCount="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Tidsperiod"/>
     <tableColumn id="2" name="22 sep 2022 - 28 sep 2022"/>
@@ -361,7 +577,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B97"/>
+  <dimension ref="A1:B169"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -960,7 +1176,7 @@
         <v>74</v>
       </c>
       <c r="B74" s="0">
-        <v>97.43</v>
+        <v>97.66</v>
       </c>
     </row>
     <row r="75">
@@ -968,7 +1184,7 @@
         <v>75</v>
       </c>
       <c r="B75" s="0">
-        <v>88.18</v>
+        <v>88.38</v>
       </c>
     </row>
     <row r="76">
@@ -976,7 +1192,7 @@
         <v>76</v>
       </c>
       <c r="B76" s="0">
-        <v>86.16</v>
+        <v>86.36</v>
       </c>
     </row>
     <row r="77">
@@ -984,7 +1200,7 @@
         <v>77</v>
       </c>
       <c r="B77" s="0">
-        <v>84.88</v>
+        <v>85.08</v>
       </c>
     </row>
     <row r="78">
@@ -992,7 +1208,7 @@
         <v>78</v>
       </c>
       <c r="B78" s="0">
-        <v>88.61</v>
+        <v>88.81</v>
       </c>
     </row>
     <row r="79">
@@ -1000,7 +1216,7 @@
         <v>79</v>
       </c>
       <c r="B79" s="0">
-        <v>128.05</v>
+        <v>128.35</v>
       </c>
     </row>
     <row r="80">
@@ -1008,7 +1224,7 @@
         <v>80</v>
       </c>
       <c r="B80" s="0">
-        <v>133.74</v>
+        <v>134.05</v>
       </c>
     </row>
     <row r="81">
@@ -1016,7 +1232,7 @@
         <v>81</v>
       </c>
       <c r="B81" s="0">
-        <v>149.45</v>
+        <v>149.8</v>
       </c>
     </row>
     <row r="82">
@@ -1024,7 +1240,7 @@
         <v>82</v>
       </c>
       <c r="B82" s="0">
-        <v>213.7</v>
+        <v>214.2</v>
       </c>
     </row>
     <row r="83">
@@ -1032,7 +1248,7 @@
         <v>83</v>
       </c>
       <c r="B83" s="0">
-        <v>234.62</v>
+        <v>235.16</v>
       </c>
     </row>
     <row r="84">
@@ -1040,7 +1256,7 @@
         <v>84</v>
       </c>
       <c r="B84" s="0">
-        <v>266.31</v>
+        <v>266.93</v>
       </c>
     </row>
     <row r="85">
@@ -1048,7 +1264,7 @@
         <v>85</v>
       </c>
       <c r="B85" s="0">
-        <v>277.63</v>
+        <v>278.28</v>
       </c>
     </row>
     <row r="86">
@@ -1056,7 +1272,7 @@
         <v>86</v>
       </c>
       <c r="B86" s="0">
-        <v>235.96</v>
+        <v>236.5</v>
       </c>
     </row>
     <row r="87">
@@ -1064,7 +1280,7 @@
         <v>87</v>
       </c>
       <c r="B87" s="0">
-        <v>249.38</v>
+        <v>249.96</v>
       </c>
     </row>
     <row r="88">
@@ -1072,7 +1288,7 @@
         <v>88</v>
       </c>
       <c r="B88" s="0">
-        <v>225.81</v>
+        <v>226.33</v>
       </c>
     </row>
     <row r="89">
@@ -1080,7 +1296,7 @@
         <v>89</v>
       </c>
       <c r="B89" s="0">
-        <v>233.55</v>
+        <v>234.09</v>
       </c>
     </row>
     <row r="90">
@@ -1088,7 +1304,7 @@
         <v>90</v>
       </c>
       <c r="B90" s="0">
-        <v>251.11</v>
+        <v>251.69</v>
       </c>
     </row>
     <row r="91">
@@ -1096,7 +1312,7 @@
         <v>91</v>
       </c>
       <c r="B91" s="0">
-        <v>350.58</v>
+        <v>351.4</v>
       </c>
     </row>
     <row r="92">
@@ -1104,7 +1320,7 @@
         <v>92</v>
       </c>
       <c r="B92" s="0">
-        <v>384.4</v>
+        <v>385.29</v>
       </c>
     </row>
     <row r="93">
@@ -1112,7 +1328,7 @@
         <v>93</v>
       </c>
       <c r="B93" s="0">
-        <v>391.45</v>
+        <v>392.36</v>
       </c>
     </row>
     <row r="94">
@@ -1120,7 +1336,7 @@
         <v>94</v>
       </c>
       <c r="B94" s="0">
-        <v>351.24</v>
+        <v>352.05</v>
       </c>
     </row>
     <row r="95">
@@ -1128,7 +1344,7 @@
         <v>95</v>
       </c>
       <c r="B95" s="0">
-        <v>233.85</v>
+        <v>234.4</v>
       </c>
     </row>
     <row r="96">
@@ -1136,7 +1352,7 @@
         <v>96</v>
       </c>
       <c r="B96" s="0">
-        <v>133.72</v>
+        <v>134.03</v>
       </c>
     </row>
     <row r="97">
@@ -1144,7 +1360,583 @@
         <v>97</v>
       </c>
       <c r="B97" s="0">
-        <v>46.97</v>
+        <v>47.08</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="B98" s="0">
+        <v>137.18</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="B99" s="0">
+        <v>66.48</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="B100" s="0">
+        <v>58.56</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" s="0" t="s">
+        <v>101</v>
+      </c>
+      <c r="B101" s="0">
+        <v>61.53</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="B102" s="0">
+        <v>86.76</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" s="0" t="s">
+        <v>103</v>
+      </c>
+      <c r="B103" s="0">
+        <v>131.65</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B104" s="0">
+        <v>64.56</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="B105" s="0">
+        <v>357.57</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="B106" s="0">
+        <v>362.08</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" s="0" t="s">
+        <v>107</v>
+      </c>
+      <c r="B107" s="0">
+        <v>319.85</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B108" s="0">
+        <v>285.01</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B109" s="0">
+        <v>238.63</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="B110" s="0">
+        <v>178.83</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B111" s="0">
+        <v>186.27</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B112" s="0">
+        <v>102.67</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" s="0" t="s">
+        <v>113</v>
+      </c>
+      <c r="B113" s="0">
+        <v>67.8</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B114" s="0">
+        <v>56.51</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B115" s="0">
+        <v>61.76</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B116" s="0">
+        <v>70.08</v>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B117" s="0">
+        <v>69.75</v>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B118" s="0">
+        <v>58.68</v>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B119" s="0">
+        <v>46.51</v>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B120" s="0">
+        <v>34.66</v>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B121" s="0">
+        <v>20.6</v>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="B122" s="0">
+        <v>15.22</v>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="B123" s="0">
+        <v>14.21</v>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B124" s="0">
+        <v>13.84</v>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" s="0" t="s">
+        <v>125</v>
+      </c>
+      <c r="B125" s="0">
+        <v>14.18</v>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B126" s="0">
+        <v>15.65</v>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B127" s="0">
+        <v>17.71</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B128" s="0">
+        <v>27.02</v>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B129" s="0">
+        <v>64.93</v>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B130" s="0">
+        <v>98.54</v>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B131" s="0">
+        <v>76.45</v>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B132" s="0">
+        <v>75.73</v>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B133" s="0">
+        <v>75.15</v>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B134" s="0">
+        <v>67.83</v>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B135" s="0">
+        <v>66.52</v>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="B136" s="0">
+        <v>63.92</v>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="0" t="s">
+        <v>137</v>
+      </c>
+      <c r="B137" s="0">
+        <v>62.76</v>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B138" s="0">
+        <v>63.45</v>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" s="0" t="s">
+        <v>139</v>
+      </c>
+      <c r="B139" s="0">
+        <v>67.82</v>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="B140" s="0">
+        <v>72.5</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B141" s="0">
+        <v>71.22</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="B142" s="0">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" s="0" t="s">
+        <v>143</v>
+      </c>
+      <c r="B143" s="0">
+        <v>57.24</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="B144" s="0">
+        <v>50.39</v>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B145" s="0">
+        <v>37.96</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B146" s="0">
+        <v>49.5</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B147" s="0">
+        <v>49.06</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B148" s="0">
+        <v>49.76</v>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B149" s="0">
+        <v>50.72</v>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B150" s="0">
+        <v>51.09</v>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B151" s="0">
+        <v>54.99</v>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B152" s="0">
+        <v>61.35</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B153" s="0">
+        <v>74.97</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B154" s="0">
+        <v>82.83</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B155" s="0">
+        <v>83.9</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B156" s="0">
+        <v>83.08</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B157" s="0">
+        <v>82.92</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B158" s="0">
+        <v>82.65</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B159" s="0">
+        <v>83.02</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B160" s="0">
+        <v>83.43</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B161" s="0">
+        <v>83.5</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="0" t="s">
+        <v>162</v>
+      </c>
+      <c r="B162" s="0">
+        <v>78.44</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B163" s="0">
+        <v>82.46</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="0" t="s">
+        <v>164</v>
+      </c>
+      <c r="B164" s="0">
+        <v>82.24</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="0" t="s">
+        <v>165</v>
+      </c>
+      <c r="B165" s="0">
+        <v>82.13</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="0" t="s">
+        <v>166</v>
+      </c>
+      <c r="B166" s="0">
+        <v>83.38</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="B167" s="0">
+        <v>76.3</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="0" t="s">
+        <v>168</v>
+      </c>
+      <c r="B168" s="0">
+        <v>76.03</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B169" s="0">
+        <v>65.36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>